<commit_message>
Updated sprint document and incorporated SphereGeometry.js file into my project.
</commit_message>
<xml_diff>
--- a/final+project.xlsx
+++ b/final+project.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernardjohn.paner\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernardjohn.paner\Desktop\Graphics_Apps_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
   <si>
     <t>Your Name:</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>I don't have to shuffle the cube myself</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>A 3D graphics application designed to emulate a Rubiks Cube rendered in a browser using HTML, Javascript, and the Three.js library. Ideally, the player will be able to manipulate distinct rows and columns of a 3D object as though it were the genuine article</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -323,13 +335,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -337,19 +355,19 @@
   </cellStyles>
   <dxfs count="49">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -503,103 +521,103 @@
     <sortCondition ref="B8:B20"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="UserStory#" dataDxfId="46"/>
-    <tableColumn id="6" name="StoryName" dataDxfId="45"/>
-    <tableColumn id="2" name="As a …" dataDxfId="44"/>
-    <tableColumn id="3" name="I want…" dataDxfId="43"/>
-    <tableColumn id="4" name="So That…" dataDxfId="42"/>
-    <tableColumn id="5" name="Status" dataDxfId="41"/>
+    <tableColumn id="1" name="UserStory#" dataDxfId="5"/>
+    <tableColumn id="6" name="StoryName" dataDxfId="4"/>
+    <tableColumn id="2" name="As a …" dataDxfId="3"/>
+    <tableColumn id="3" name="I want…" dataDxfId="2"/>
+    <tableColumn id="4" name="So That…" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:H13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:H13" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="B4:H13"/>
   <sortState ref="B5:H13">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="12" name="Priority" dataDxfId="38"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="37"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="36"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="35"/>
-    <tableColumn id="3" name="Description" dataDxfId="34"/>
-    <tableColumn id="4" name="In" dataDxfId="33"/>
-    <tableColumn id="8" name="InSprint" dataDxfId="32"/>
+    <tableColumn id="12" name="Priority" dataDxfId="44"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="43"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="42"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="41"/>
+    <tableColumn id="3" name="Description" dataDxfId="40"/>
+    <tableColumn id="4" name="In" dataDxfId="39"/>
+    <tableColumn id="8" name="InSprint" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="B3:G12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="B3:G12" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" name="Points" dataDxfId="29"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="28"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="27"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="26"/>
-    <tableColumn id="3" name="Description" dataDxfId="25"/>
-    <tableColumn id="4" name="In" dataDxfId="24"/>
+    <tableColumn id="12" name="Points" dataDxfId="35"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="34"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="33"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="32"/>
+    <tableColumn id="3" name="Description" dataDxfId="31"/>
+    <tableColumn id="4" name="In" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B3:G12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B3:G12" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" name="Points" dataDxfId="21"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="20"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="19"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="18"/>
-    <tableColumn id="3" name="Description" dataDxfId="17"/>
-    <tableColumn id="4" name="In" dataDxfId="16"/>
+    <tableColumn id="12" name="Points" dataDxfId="27"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="26"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="25"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="24"/>
+    <tableColumn id="3" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" name="In" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table246" displayName="Table246" ref="B3:G12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table246" displayName="Table246" ref="B3:G12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" name="Points" dataDxfId="13"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="12"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="11"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="10"/>
-    <tableColumn id="3" name="Description" dataDxfId="9"/>
-    <tableColumn id="4" name="In" dataDxfId="8"/>
+    <tableColumn id="12" name="Points" dataDxfId="19"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="18"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="17"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="16"/>
+    <tableColumn id="3" name="Description" dataDxfId="15"/>
+    <tableColumn id="4" name="In" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table247" displayName="Table247" ref="B3:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table247" displayName="Table247" ref="B3:G12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B3:G12"/>
   <sortState ref="B4:H12">
     <sortCondition descending="1" ref="B19:B28"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" name="Points" dataDxfId="5"/>
-    <tableColumn id="10" name="BacklogId" dataDxfId="4"/>
-    <tableColumn id="1" name="StoryName" dataDxfId="3"/>
-    <tableColumn id="2" name="BacklogType" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" name="In" dataDxfId="0"/>
+    <tableColumn id="12" name="Points" dataDxfId="11"/>
+    <tableColumn id="10" name="BacklogId" dataDxfId="10"/>
+    <tableColumn id="1" name="StoryName" dataDxfId="9"/>
+    <tableColumn id="2" name="BacklogType" dataDxfId="8"/>
+    <tableColumn id="3" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" name="In" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,7 +889,7 @@
   <dimension ref="C3:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,68 +905,70 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -962,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +994,8 @@
     <col min="4" max="4" width="58.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="69.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="61.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="11.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="7" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
@@ -1006,203 +1027,233 @@
       <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="10" t="s">
         <v>69</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="11" t="s">
         <v>59</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="10" t="s">
         <v>44</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="10" t="s">
         <v>43</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="10" t="s">
         <v>60</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>5</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="10" t="s">
         <v>45</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="10" t="s">
         <v>46</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>7</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="10" t="s">
         <v>47</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>9</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>10</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>11</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1277,7 @@
   <dimension ref="B3:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B5" sqref="B5:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,14 +1478,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="71.42578125" customWidth="1"/>
+    <col min="6" max="6" width="79.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1464,68 +1515,92 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="F6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>

</xml_diff>